<commit_message>
Add ui image support.
</commit_message>
<xml_diff>
--- a/Assets/Wugner/Localization/Examples/TestExcel.xlsx
+++ b/Assets/Wugner/Localization/Examples/TestExcel.xlsx
@@ -29,14 +29,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FONT_zh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CONTENT_zh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CONTENT_en</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -97,6 +89,14 @@
   </si>
   <si>
     <t>Common button for next step in navigation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CONTENT_cn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FONT_cn</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -428,7 +428,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -445,25 +445,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>1</v>
@@ -471,49 +471,49 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B38" xr:uid="{6BE1920A-51E9-480B-973A-94947B295C35}">
-      <formula1>"Text,Sprite"</formula1>
+      <formula1>"Text,Image"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>